<commit_message>
change a bunch thins i think
</commit_message>
<xml_diff>
--- a/Archive/colonial_transit_time_20250828.xlsx
+++ b/Archive/colonial_transit_time_20250828.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statoilsrm-my.sharepoint.com/personal/siwz_equinor_com/Documents/personal/projects/Colonial Pipeline Forecast/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://statoilsrm-my.sharepoint.com/personal/siwz_equinor_com/Documents/personal/projects/colonial_forecast/Archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_8AA6420ECBA85BE38963B671F3375B06C4986908" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8DC9A80-3432-4ADA-BD8A-B83B0F5BCA37}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_8AA6420ECBA85BE38963B671F3375B06C4986908" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F61A3CB-7451-45A8-B610-881ED0421A9B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13110,8 +13110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1FC39A-7D82-442F-BDFD-587844FC7A7C}">
   <dimension ref="A1:H302"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>